<commit_message>
add check sheet comment
</commit_message>
<xml_diff>
--- a/src/main/resources/root/en/check_sheet.xlsx
+++ b/src/main/resources/root/en/check_sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="9435" activeTab="1"/>
+    <workbookView windowWidth="28695" windowHeight="14820"/>
   </bookViews>
   <sheets>
     <sheet name="Target" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189">
   <si>
     <t>項目ID</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>RuleDB</t>
+  </si>
+  <si>
+    <t>以降の行はユーザ定義パラメータの指定行となり、検査コード、検査ルールからserver_info['項目ID']パラメータで値を参照します</t>
   </si>
   <si>
     <t>ID</t>
@@ -306,13 +309,13 @@
     <t>mem_total</t>
   </si>
   <si>
-    <t>物理搭載メモリ量[MB]</t>
+    <t>物理搭載メモリ量[KB]</t>
   </si>
   <si>
     <t>mem_free</t>
   </si>
   <si>
-    <t>メモリ空き容量[MB]</t>
+    <t>メモリ空き容量[KB]</t>
   </si>
   <si>
     <t>network</t>
@@ -547,7 +550,7 @@
     <t>free_physical</t>
   </si>
   <si>
-    <t>空きメモリ量[MB]</t>
+    <t>空きメモリ量[KB]</t>
   </si>
   <si>
     <t>driver</t>
@@ -602,7 +605,7 @@
     <numFmt numFmtId="177" formatCode="_-&quot;\&quot;* #,##0.00_-\ ;\-&quot;\&quot;* #,##0.00_-\ ;_-&quot;\&quot;* &quot;-&quot;??_-\ ;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -625,29 +628,8 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="メイリオ"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Meiryo UI"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -658,20 +640,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -688,7 +662,67 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -702,19 +736,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -734,54 +760,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -794,17 +775,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -817,7 +792,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -835,13 +816,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -859,7 +900,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -871,79 +936,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -961,37 +960,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1048,17 +1023,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1070,6 +1034,39 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1093,31 +1090,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1139,184 +1112,186 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="56">
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="29">
       <alignment vertical="center"/>
     </xf>
@@ -1350,28 +1325,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="47" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="23" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="23" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="11" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="23" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="23" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="11" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="47" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="29" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="29" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="11" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="29" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="29" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1727,307 +1699,309 @@
   <sheetPr/>
   <dimension ref="B4:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="36.875" customWidth="1"/>
-    <col min="4" max="8" width="14.5" customWidth="1"/>
-    <col min="9" max="9" width="12.25" customWidth="1"/>
+    <col min="3" max="3" width="36.8761904761905" customWidth="1"/>
+    <col min="4" max="8" width="14.5047619047619" customWidth="1"/>
+    <col min="9" max="9" width="12.247619047619" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:13">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <v>1</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="16">
         <v>2</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="16">
         <v>3</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="16">
         <v>4</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="16">
         <v>5</v>
       </c>
-      <c r="I4" s="17">
+      <c r="I4" s="16">
         <v>6</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="16">
         <v>7</v>
       </c>
-      <c r="K4" s="17">
+      <c r="K4" s="16">
         <v>8</v>
       </c>
-      <c r="L4" s="17">
+      <c r="L4" s="16">
         <v>9</v>
       </c>
-      <c r="M4" s="17">
+      <c r="M4" s="16">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:13">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-    </row>
-    <row r="6" ht="24.75" spans="2:13">
-      <c r="B6" s="17" t="s">
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+    </row>
+    <row r="6" ht="28.5" spans="2:13">
+      <c r="B6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-    </row>
-    <row r="7" ht="25.5" spans="2:13">
-      <c r="B7" s="17" t="s">
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+    </row>
+    <row r="7" ht="28.5" spans="2:13">
+      <c r="B7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-    </row>
-    <row r="8" ht="63" spans="2:13">
-      <c r="B8" s="17" t="s">
+      <c r="E7" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+    </row>
+    <row r="8" ht="71.25" spans="2:13">
+      <c r="B8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-    </row>
-    <row r="9" ht="49.5" spans="2:13">
-      <c r="B9" s="17" t="s">
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+    </row>
+    <row r="9" ht="57" spans="2:13">
+      <c r="B9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-    </row>
-    <row r="10" ht="36.75" spans="2:13">
-      <c r="B10" s="17" t="s">
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+    </row>
+    <row r="10" ht="42.75" spans="2:13">
+      <c r="B10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-    </row>
-    <row r="11" ht="24.75" spans="2:13">
-      <c r="B11" s="17" t="s">
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+    </row>
+    <row r="11" ht="28.5" spans="2:13">
+      <c r="B11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-    </row>
-    <row r="12" spans="2:13">
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+    </row>
+    <row r="12" ht="42.75" spans="2:13">
+      <c r="B12" s="16"/>
+      <c r="C12" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
     </row>
     <row r="13" spans="2:13">
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
     </row>
     <row r="14" spans="2:13">
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
     </row>
     <row r="15" spans="2:13">
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
     </row>
     <row r="16" spans="2:13">
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
     </row>
     <row r="17" spans="2:13">
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
     </row>
     <row r="18" spans="2:13">
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2041,18 +2015,18 @@
   <sheetPr/>
   <dimension ref="A4:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="2" max="2" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="20.6285714285714" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="9.75" customWidth="1"/>
-    <col min="5" max="5" width="6.5" customWidth="1"/>
-    <col min="6" max="6" width="54.875" customWidth="1"/>
-    <col min="7" max="10" width="14.375" customWidth="1"/>
+    <col min="4" max="4" width="9.75238095238095" customWidth="1"/>
+    <col min="5" max="5" width="6.5047619047619" customWidth="1"/>
+    <col min="6" max="6" width="54.8761904761905" customWidth="1"/>
+    <col min="7" max="10" width="14.3714285714286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:6">
@@ -2060,403 +2034,403 @@
         <v>15</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="8"/>
       <c r="B6" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="8"/>
       <c r="B7" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="8"/>
       <c r="B8" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="8"/>
       <c r="B9" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="8"/>
       <c r="B10" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="10" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" ht="28.5" spans="1:6">
       <c r="A19" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="8"/>
       <c r="B20" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="8"/>
       <c r="B21" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="8"/>
       <c r="B22" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="8"/>
       <c r="B23" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="8"/>
       <c r="B24" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" ht="42.75" spans="1:6">
       <c r="A25" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" ht="28.5" spans="1:6">
       <c r="A26" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="8"/>
       <c r="B27" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9" t="s">
@@ -2464,13 +2438,13 @@
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="8"/>
       <c r="B28" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9" t="s">
@@ -2478,179 +2452,179 @@
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" ht="28.5" spans="1:6">
       <c r="A29" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="8"/>
       <c r="B30" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" ht="28.5" spans="1:6">
       <c r="A31" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" ht="42.75" spans="1:6">
       <c r="A32" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" ht="42.75" spans="1:6">
       <c r="A33" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E33" s="9"/>
       <c r="F33" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" ht="71.25" spans="1:6">
       <c r="A34" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" ht="42.75" spans="1:6">
       <c r="A35" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E35" s="9"/>
       <c r="F35" s="10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="9"/>
       <c r="F36" s="10" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="38" ht="28.5" spans="1:6">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" ht="42.75" spans="1:6">
       <c r="A38" s="9"/>
       <c r="B38" s="9" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="9" t="s">
@@ -2658,233 +2632,233 @@
       </c>
       <c r="E38" s="9"/>
       <c r="F38" s="10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="39" ht="16.5" spans="1:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="C39" s="11" t="s">
         <v>128</v>
       </c>
+      <c r="C39" s="9" t="s">
+        <v>129</v>
+      </c>
       <c r="D39" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E39" s="9"/>
-      <c r="F39" s="12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="40" ht="33" spans="1:6">
+      <c r="F39" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" ht="28.5" spans="1:6">
       <c r="A40" s="9"/>
       <c r="B40" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C40" s="11" t="s">
         <v>131</v>
       </c>
+      <c r="C40" s="9" t="s">
+        <v>132</v>
+      </c>
       <c r="D40" s="9" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="9"/>
-      <c r="F40" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="41" ht="16.5" spans="1:6">
-      <c r="A41" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B41" s="13" t="s">
+      <c r="F40" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C41" s="11" t="s">
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" s="11" t="s">
         <v>134</v>
       </c>
+      <c r="C41" s="9" t="s">
+        <v>135</v>
+      </c>
       <c r="D41" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E41" s="13"/>
-      <c r="F41" s="12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="42" ht="16.5" spans="1:6">
-      <c r="A42" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B42" s="13" t="s">
+      <c r="E41" s="11"/>
+      <c r="F41" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="C42" s="11" t="s">
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="11" t="s">
         <v>137</v>
       </c>
+      <c r="C42" s="9" t="s">
+        <v>138</v>
+      </c>
       <c r="D42" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E42" s="13"/>
-      <c r="F42" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="43" ht="16.5" spans="1:6">
-      <c r="A43" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" s="13" t="s">
+      <c r="E42" s="11"/>
+      <c r="F42" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C43" s="11" t="s">
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="11" t="s">
         <v>140</v>
       </c>
+      <c r="C43" s="9" t="s">
+        <v>141</v>
+      </c>
       <c r="D43" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E43" s="13"/>
-      <c r="F43" s="12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="44" ht="33" spans="1:6">
-      <c r="A44" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44" s="13" t="s">
+      <c r="E43" s="11"/>
+      <c r="F43" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="C44" s="11" t="s">
+    </row>
+    <row r="44" ht="28.5" spans="1:6">
+      <c r="A44" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="11" t="s">
         <v>143</v>
       </c>
+      <c r="C44" s="9" t="s">
+        <v>144</v>
+      </c>
       <c r="D44" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E44" s="13"/>
-      <c r="F44" s="12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="45" ht="49.5" spans="1:6">
-      <c r="A45" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" s="13" t="s">
+      <c r="E44" s="11"/>
+      <c r="F44" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="C45" s="11" t="s">
+    </row>
+    <row r="45" ht="42.75" spans="1:6">
+      <c r="A45" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" s="11" t="s">
         <v>146</v>
       </c>
+      <c r="C45" s="9" t="s">
+        <v>147</v>
+      </c>
       <c r="D45" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E45" s="13"/>
-      <c r="F45" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="46" ht="33" spans="1:6">
-      <c r="A46" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B46" s="13" t="s">
+      <c r="E45" s="11"/>
+      <c r="F45" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C46" s="11" t="s">
+    </row>
+    <row r="46" ht="28.5" spans="1:6">
+      <c r="A46" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="11" t="s">
         <v>149</v>
       </c>
+      <c r="C46" s="9" t="s">
+        <v>150</v>
+      </c>
       <c r="D46" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E46" s="13"/>
-      <c r="F46" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="47" ht="16.5" spans="1:6">
-      <c r="A47" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B47" s="13" t="s">
+      <c r="E46" s="11"/>
+      <c r="F46" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="C47" s="11" t="s">
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B47" s="11" t="s">
         <v>152</v>
       </c>
+      <c r="C47" s="9" t="s">
+        <v>153</v>
+      </c>
       <c r="D47" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="48" ht="16.5" spans="1:6">
-      <c r="A48" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B48" s="13" t="s">
+      <c r="E47" s="11"/>
+      <c r="F47" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="C48" s="11" t="s">
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B48" s="11" t="s">
         <v>155</v>
       </c>
+      <c r="C48" s="9" t="s">
+        <v>156</v>
+      </c>
       <c r="D48" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E48" s="13"/>
-      <c r="F48" s="12" t="s">
-        <v>156</v>
+      <c r="E48" s="11"/>
+      <c r="F48" s="10" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="13"/>
-      <c r="B49" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="C49" s="13"/>
+      <c r="A49" s="11"/>
+      <c r="B49" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C49" s="11"/>
       <c r="D49" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="50" ht="33" spans="1:6">
-      <c r="A50" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B50" s="13" t="s">
+      <c r="E49" s="11"/>
+      <c r="F49" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="C50" s="11" t="s">
+    </row>
+    <row r="50" ht="28.5" spans="1:6">
+      <c r="A50" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50" s="11" t="s">
         <v>160</v>
       </c>
+      <c r="C50" s="9" t="s">
+        <v>161</v>
+      </c>
       <c r="D50" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E50" s="13"/>
-      <c r="F50" s="12" t="s">
-        <v>161</v>
+      <c r="E50" s="11"/>
+      <c r="F50" s="10" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E51" s="15"/>
+      <c r="A51" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C51" s="13"/>
+      <c r="D51" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E51" s="13"/>
       <c r="F51" s="15" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2900,17 +2874,17 @@
   <dimension ref="A4:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:F14"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col min="2" max="2" width="17.625" customWidth="1"/>
-    <col min="3" max="3" width="27.25" customWidth="1"/>
-    <col min="4" max="4" width="15.75" customWidth="1"/>
-    <col min="5" max="5" width="6.5" customWidth="1"/>
-    <col min="6" max="6" width="56.625" customWidth="1"/>
-    <col min="7" max="7" width="15.125" customWidth="1"/>
+    <col min="2" max="2" width="17.6285714285714" customWidth="1"/>
+    <col min="3" max="3" width="27.247619047619" customWidth="1"/>
+    <col min="4" max="4" width="15.752380952381" customWidth="1"/>
+    <col min="5" max="5" width="6.5047619047619" customWidth="1"/>
+    <col min="6" max="6" width="56.6285714285714" customWidth="1"/>
+    <col min="7" max="7" width="15.1238095238095" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="1:6">
@@ -2918,291 +2892,291 @@
         <v>15</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="8"/>
       <c r="B16" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="8"/>
       <c r="B17" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="8"/>
       <c r="B18" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="10" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" ht="28.5" spans="1:6">
       <c r="A19" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="10" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="8"/>
       <c r="B20" s="9" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9" t="s">
@@ -3210,13 +3184,13 @@
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="8"/>
       <c r="B21" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9" t="s">
@@ -3224,101 +3198,101 @@
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="10" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" ht="28.5" spans="1:6">
       <c r="A22" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="10" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="10" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" ht="28.5" spans="1:6">
       <c r="A25" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>11</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3405,21 +3379,21 @@
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="9.75" customWidth="1"/>
-    <col min="5" max="5" width="16.125" customWidth="1"/>
-    <col min="6" max="6" width="16.25" customWidth="1"/>
+    <col min="4" max="4" width="9.75238095238095" customWidth="1"/>
+    <col min="5" max="5" width="16.1238095238095" customWidth="1"/>
+    <col min="6" max="6" width="16.247619047619" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" ht="18.75" spans="1:6">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>22</v>
@@ -3431,13 +3405,13 @@
     <row r="5" ht="18.75" spans="1:6">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -3445,13 +3419,13 @@
     <row r="6" ht="18.75" spans="1:6">
       <c r="A6" s="4"/>
       <c r="B6" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -3459,13 +3433,13 @@
     <row r="7" ht="18.75" spans="1:6">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -3473,13 +3447,13 @@
     <row r="8" ht="18.75" spans="1:6">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -3487,13 +3461,13 @@
     <row r="9" ht="18.75" spans="1:6">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -3501,13 +3475,13 @@
     <row r="10" ht="18.75" spans="1:6">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -3515,13 +3489,13 @@
     <row r="11" ht="18.75" spans="1:6">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -3529,10 +3503,10 @@
     <row r="12" ht="18.75" spans="1:6">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>12</v>
@@ -3543,10 +3517,10 @@
     <row r="13" ht="18.75" spans="1:6">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>12</v>
@@ -3557,10 +3531,10 @@
     <row r="14" ht="18.75" spans="1:6">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>12</v>
@@ -3571,10 +3545,10 @@
     <row r="15" ht="18.75" spans="1:6">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>12</v>
@@ -3585,10 +3559,10 @@
     <row r="16" ht="18.75" spans="1:6">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>11</v>
@@ -3599,10 +3573,10 @@
     <row r="17" ht="18.75" spans="1:6">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>11</v>
@@ -3613,10 +3587,10 @@
     <row r="18" ht="18.75" spans="1:6">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>11</v>
@@ -3627,10 +3601,10 @@
     <row r="19" ht="18.75" spans="1:6">
       <c r="A19" s="4"/>
       <c r="B19" s="5" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>11</v>
@@ -3641,10 +3615,10 @@
     <row r="20" ht="18.75" spans="1:6">
       <c r="A20" s="4"/>
       <c r="B20" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>11</v>
@@ -3655,10 +3629,10 @@
     <row r="21" ht="18.75" spans="1:6">
       <c r="A21" s="4"/>
       <c r="B21" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>11</v>
@@ -3669,10 +3643,10 @@
     <row r="22" ht="18.75" spans="1:6">
       <c r="A22" s="4"/>
       <c r="B22" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>11</v>
@@ -3683,10 +3657,10 @@
     <row r="23" ht="18.75" spans="1:6">
       <c r="A23" s="4"/>
       <c r="B23" s="5" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>11</v>

</xml_diff>